<commit_message>
Update global variables 3/14/18 10:43 AM
</commit_message>
<xml_diff>
--- a/Arm Position Spreadsheet.xlsx
+++ b/Arm Position Spreadsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\snobotics\Arm Dynamics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\981LabViewComponents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -539,6 +539,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2738,7 +2741,7 @@
     <mergeCell ref="H10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="83" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>